<commit_message>
Added Metrics to Workbooks
.
</commit_message>
<xml_diff>
--- a/Test Procedure/Symptom Checker/Chickenpox.xlsx
+++ b/Test Procedure/Symptom Checker/Chickenpox.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27510"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mason/Documents/Senior-Design-2-Electric-Boogaloo/Test Procedure/Symptom Checker/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14680"/>
   </bookViews>
   <sheets>
     <sheet name="Chickenpox" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -28,8 +41,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,14 +71,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -112,12 +131,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -144,14 +163,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -178,6 +198,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,46 +374,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I255"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N255"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>2</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+      <c r="H1">
+        <v>4</v>
+      </c>
+      <c r="I1">
+        <v>5</v>
+      </c>
+      <c r="J1">
+        <v>6</v>
+      </c>
+      <c r="K1">
+        <v>7</v>
+      </c>
+      <c r="L1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2">
+        <f>COUNTIF(B:B, "Chickenpox")</f>
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:L2" si="0">COUNTIF(C:C, "Chickenpox")</f>
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>SUM(E2:L2)</f>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <f>COUNTIF(B:B, "*")</f>
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:P3" si="1">COUNTIF(C:C, "*")</f>
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <f>SUM(E3:L3)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4" s="1">
+        <f>E2/E3</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:N4" si="2">F2/F3</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.98431372549019602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>15</v>
       </c>
@@ -400,7 +556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>31</v>
       </c>
@@ -408,7 +564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>38</v>
       </c>
@@ -416,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>66</v>
       </c>
@@ -424,7 +580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -435,7 +591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0</v>
       </c>
@@ -446,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -457,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
@@ -468,7 +624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
@@ -479,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
@@ -490,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
@@ -501,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -512,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -523,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -534,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -545,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>6</v>
       </c>
@@ -556,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>6</v>
       </c>
@@ -567,7 +723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>13</v>
       </c>
@@ -578,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>13</v>
       </c>
@@ -589,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>13</v>
       </c>
@@ -600,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>13</v>
       </c>
@@ -611,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>13</v>
       </c>
@@ -622,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>14</v>
       </c>
@@ -633,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
@@ -644,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>14</v>
       </c>
@@ -655,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>14</v>
       </c>
@@ -666,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
@@ -677,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>15</v>
       </c>
@@ -688,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>15</v>
       </c>
@@ -699,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -710,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>31</v>
       </c>
@@ -721,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>38</v>
       </c>
@@ -732,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -746,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -760,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0</v>
       </c>
@@ -774,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -788,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -802,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0</v>
       </c>
@@ -816,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0</v>
       </c>
@@ -830,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0</v>
       </c>
@@ -844,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0</v>
       </c>
@@ -858,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0</v>
       </c>
@@ -872,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0</v>
       </c>
@@ -886,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0</v>
       </c>
@@ -900,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>0</v>
       </c>
@@ -914,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0</v>
       </c>
@@ -928,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0</v>
       </c>
@@ -942,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>0</v>
       </c>
@@ -956,7 +1112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>0</v>
       </c>
@@ -970,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0</v>
       </c>
@@ -984,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0</v>
       </c>
@@ -998,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>0</v>
       </c>
@@ -1012,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>0</v>
       </c>
@@ -1026,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>6</v>
       </c>
@@ -1040,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>6</v>
       </c>
@@ -1054,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>6</v>
       </c>
@@ -1068,7 +1224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>6</v>
       </c>
@@ -1082,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>6</v>
       </c>
@@ -1096,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>6</v>
       </c>
@@ -1110,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>6</v>
       </c>
@@ -1124,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>6</v>
       </c>
@@ -1138,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>6</v>
       </c>
@@ -1152,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>6</v>
       </c>
@@ -1166,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>6</v>
       </c>
@@ -1180,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>6</v>
       </c>
@@ -1194,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>6</v>
       </c>
@@ -1208,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>6</v>
       </c>
@@ -1222,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>6</v>
       </c>
@@ -1236,7 +1392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>13</v>
       </c>
@@ -1250,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>13</v>
       </c>
@@ -1264,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>13</v>
       </c>
@@ -1278,7 +1434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>13</v>
       </c>
@@ -1292,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>13</v>
       </c>
@@ -1306,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>13</v>
       </c>
@@ -1320,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>13</v>
       </c>
@@ -1334,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>13</v>
       </c>
@@ -1348,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>13</v>
       </c>
@@ -1362,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>13</v>
       </c>
@@ -1376,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>14</v>
       </c>
@@ -1390,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>14</v>
       </c>
@@ -1404,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>14</v>
       </c>
@@ -1418,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>14</v>
       </c>
@@ -1432,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>14</v>
       </c>
@@ -1446,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>14</v>
       </c>
@@ -1460,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>15</v>
       </c>
@@ -1474,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>15</v>
       </c>
@@ -1488,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>15</v>
       </c>
@@ -1502,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>31</v>
       </c>
@@ -1516,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>0</v>
       </c>
@@ -1533,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>0</v>
       </c>
@@ -1550,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>0</v>
       </c>
@@ -1567,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>0</v>
       </c>
@@ -1584,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>0</v>
       </c>
@@ -1601,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>0</v>
       </c>
@@ -1618,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>0</v>
       </c>
@@ -1635,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>0</v>
       </c>
@@ -1652,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>0</v>
       </c>
@@ -1669,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>0</v>
       </c>
@@ -1686,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>0</v>
       </c>
@@ -1703,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>0</v>
       </c>
@@ -1720,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>0</v>
       </c>
@@ -1737,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>0</v>
       </c>
@@ -1754,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>0</v>
       </c>
@@ -1771,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>0</v>
       </c>
@@ -1788,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>0</v>
       </c>
@@ -1805,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>0</v>
       </c>
@@ -1822,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>0</v>
       </c>
@@ -1839,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>0</v>
       </c>
@@ -1856,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>0</v>
       </c>
@@ -1873,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>0</v>
       </c>
@@ -1890,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>0</v>
       </c>
@@ -1907,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>0</v>
       </c>
@@ -1924,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>0</v>
       </c>
@@ -1941,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>0</v>
       </c>
@@ -1958,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>0</v>
       </c>
@@ -1975,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>0</v>
       </c>
@@ -1992,7 +2148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>0</v>
       </c>
@@ -2009,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>0</v>
       </c>
@@ -2026,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>0</v>
       </c>
@@ -2043,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>0</v>
       </c>
@@ -2060,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>0</v>
       </c>
@@ -2077,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>0</v>
       </c>
@@ -2094,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>0</v>
       </c>
@@ -2111,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>6</v>
       </c>
@@ -2128,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>6</v>
       </c>
@@ -2145,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>6</v>
       </c>
@@ -2162,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>6</v>
       </c>
@@ -2179,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>6</v>
       </c>
@@ -2196,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>6</v>
       </c>
@@ -2213,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>6</v>
       </c>
@@ -2230,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>6</v>
       </c>
@@ -2247,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>6</v>
       </c>
@@ -2264,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>6</v>
       </c>
@@ -2281,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>6</v>
       </c>
@@ -2298,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>6</v>
       </c>
@@ -2315,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>6</v>
       </c>
@@ -2332,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>6</v>
       </c>
@@ -2349,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>6</v>
       </c>
@@ -2366,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>6</v>
       </c>
@@ -2383,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>6</v>
       </c>
@@ -2400,7 +2556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>6</v>
       </c>
@@ -2417,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>6</v>
       </c>
@@ -2434,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>6</v>
       </c>
@@ -2451,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>13</v>
       </c>
@@ -2468,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>13</v>
       </c>
@@ -2485,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>13</v>
       </c>
@@ -2502,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>13</v>
       </c>
@@ -2519,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>13</v>
       </c>
@@ -2536,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>13</v>
       </c>
@@ -2553,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>13</v>
       </c>
@@ -2570,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>13</v>
       </c>
@@ -2587,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>13</v>
       </c>
@@ -2604,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>13</v>
       </c>
@@ -2621,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>14</v>
       </c>
@@ -2638,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>14</v>
       </c>
@@ -2655,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>14</v>
       </c>
@@ -2672,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>14</v>
       </c>
@@ -2689,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>15</v>
       </c>
@@ -2706,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>0</v>
       </c>
@@ -2726,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>0</v>
       </c>
@@ -2746,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>0</v>
       </c>
@@ -2766,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>0</v>
       </c>
@@ -2786,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>0</v>
       </c>
@@ -2806,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>0</v>
       </c>
@@ -2826,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>0</v>
       </c>
@@ -2846,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>0</v>
       </c>
@@ -2866,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>0</v>
       </c>
@@ -2886,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>0</v>
       </c>
@@ -2906,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>0</v>
       </c>
@@ -2926,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>0</v>
       </c>
@@ -2946,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>0</v>
       </c>
@@ -2966,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>0</v>
       </c>
@@ -2986,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>0</v>
       </c>
@@ -3006,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>0</v>
       </c>
@@ -3026,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>0</v>
       </c>
@@ -3046,7 +3202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>0</v>
       </c>
@@ -3066,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>0</v>
       </c>
@@ -3086,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>0</v>
       </c>
@@ -3106,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>0</v>
       </c>
@@ -3126,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>0</v>
       </c>
@@ -3146,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>0</v>
       </c>
@@ -3166,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>0</v>
       </c>
@@ -3186,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>0</v>
       </c>
@@ -3206,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>0</v>
       </c>
@@ -3226,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>0</v>
       </c>
@@ -3246,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>0</v>
       </c>
@@ -3266,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>0</v>
       </c>
@@ -3286,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>0</v>
       </c>
@@ -3306,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>0</v>
       </c>
@@ -3326,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>0</v>
       </c>
@@ -3346,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>0</v>
       </c>
@@ -3366,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>0</v>
       </c>
@@ -3386,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>0</v>
       </c>
@@ -3406,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>6</v>
       </c>
@@ -3426,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>6</v>
       </c>
@@ -3446,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>6</v>
       </c>
@@ -3466,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>6</v>
       </c>
@@ -3486,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>6</v>
       </c>
@@ -3506,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>6</v>
       </c>
@@ -3526,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>6</v>
       </c>
@@ -3546,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>6</v>
       </c>
@@ -3566,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>6</v>
       </c>
@@ -3586,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>6</v>
       </c>
@@ -3606,7 +3762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>6</v>
       </c>
@@ -3626,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>6</v>
       </c>
@@ -3646,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>6</v>
       </c>
@@ -3666,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>6</v>
       </c>
@@ -3686,7 +3842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>6</v>
       </c>
@@ -3706,7 +3862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>13</v>
       </c>
@@ -3726,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:7">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>13</v>
       </c>
@@ -3746,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>13</v>
       </c>
@@ -3766,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>13</v>
       </c>
@@ -3786,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>13</v>
       </c>
@@ -3806,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>14</v>
       </c>
@@ -3826,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>0</v>
       </c>
@@ -3849,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>0</v>
       </c>
@@ -3872,7 +4028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>0</v>
       </c>
@@ -3895,7 +4051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>0</v>
       </c>
@@ -3918,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>0</v>
       </c>
@@ -3941,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>0</v>
       </c>
@@ -3964,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>0</v>
       </c>
@@ -3987,7 +4143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>0</v>
       </c>
@@ -4010,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>0</v>
       </c>
@@ -4033,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>0</v>
       </c>
@@ -4056,7 +4212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>0</v>
       </c>
@@ -4079,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>0</v>
       </c>
@@ -4102,7 +4258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>0</v>
       </c>
@@ -4125,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>0</v>
       </c>
@@ -4148,7 +4304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>0</v>
       </c>
@@ -4171,7 +4327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>0</v>
       </c>
@@ -4194,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>0</v>
       </c>
@@ -4217,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>0</v>
       </c>
@@ -4240,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>0</v>
       </c>
@@ -4263,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>0</v>
       </c>
@@ -4286,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>0</v>
       </c>
@@ -4309,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>6</v>
       </c>
@@ -4332,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>6</v>
       </c>
@@ -4355,7 +4511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>6</v>
       </c>
@@ -4378,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>6</v>
       </c>
@@ -4401,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>6</v>
       </c>
@@ -4424,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>6</v>
       </c>
@@ -4447,7 +4603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>13</v>
       </c>
@@ -4470,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>0</v>
       </c>
@@ -4496,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>0</v>
       </c>
@@ -4522,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>0</v>
       </c>
@@ -4548,7 +4704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>0</v>
       </c>
@@ -4574,7 +4730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>0</v>
       </c>
@@ -4600,7 +4756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>0</v>
       </c>
@@ -4626,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>0</v>
       </c>
@@ -4652,7 +4808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>6</v>
       </c>
@@ -4678,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>0</v>
       </c>

</xml_diff>